<commit_message>
Added Correction value to compensate for projectile diameter.
</commit_message>
<xml_diff>
--- a/HyperbolaCalc.xlsx
+++ b/HyperbolaCalc.xlsx
@@ -9,15 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="B_H1">Sheet1!$K$14</definedName>
     <definedName name="B_H2">Sheet1!$O$14</definedName>
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Width</t>
   </si>
@@ -125,13 +122,35 @@
   <si>
     <t>Height</t>
   </si>
+  <si>
+    <t>Clock Speed</t>
+  </si>
+  <si>
+    <t>Pre-scaler</t>
+  </si>
+  <si>
+    <t>Speed of sound</t>
+  </si>
+  <si>
+    <t>mm/count</t>
+  </si>
+  <si>
+    <t>seconds per count</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>mm per count</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -162,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -176,6 +195,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,4425 +211,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="F3">
-            <v>520.39840807808514</v>
-          </cell>
-          <cell r="H3">
-            <v>1202.1565996158736</v>
-          </cell>
-          <cell r="I3">
-            <v>396</v>
-          </cell>
-          <cell r="J3">
-            <v>533.66775124910134</v>
-          </cell>
-          <cell r="L3">
-            <v>1416.9835212107148</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="F4">
-            <v>520.34008825802653</v>
-          </cell>
-          <cell r="H4">
-            <v>1194.6632203261302</v>
-          </cell>
-          <cell r="I4">
-            <v>397</v>
-          </cell>
-          <cell r="J4">
-            <v>533.61992195945697</v>
-          </cell>
-          <cell r="L4">
-            <v>1408.6245951281696</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="F5">
-            <v>520.28166704405578</v>
-          </cell>
-          <cell r="H5">
-            <v>1187.160650459743</v>
-          </cell>
-          <cell r="I5">
-            <v>398</v>
-          </cell>
-          <cell r="J5">
-            <v>533.57200942309942</v>
-          </cell>
-          <cell r="L5">
-            <v>1400.2582577052008</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="F6">
-            <v>520.22314467382182</v>
-          </cell>
-          <cell r="H6">
-            <v>1179.6487146604279</v>
-          </cell>
-          <cell r="I6">
-            <v>399</v>
-          </cell>
-          <cell r="J6">
-            <v>533.52401383466872</v>
-          </cell>
-          <cell r="L6">
-            <v>1391.8843752975786</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="F7">
-            <v>520.1645213846416</v>
-          </cell>
-          <cell r="H7">
-            <v>1172.1272328548637</v>
-          </cell>
-          <cell r="I7">
-            <v>400</v>
-          </cell>
-          <cell r="J7">
-            <v>533.47593538853448</v>
-          </cell>
-          <cell r="L7">
-            <v>1383.5028109034611</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="F8">
-            <v>520.1057974134975</v>
-          </cell>
-          <cell r="H8">
-            <v>1164.5960200859352</v>
-          </cell>
-          <cell r="I8">
-            <v>401</v>
-          </cell>
-          <cell r="J8">
-            <v>533.42777427879389</v>
-          </cell>
-          <cell r="L8">
-            <v>1375.1134240535744</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="F9">
-            <v>520.04697299703537</v>
-          </cell>
-          <cell r="H9">
-            <v>1157.0548863385868</v>
-          </cell>
-          <cell r="I9">
-            <v>402</v>
-          </cell>
-          <cell r="J9">
-            <v>533.37953069927084</v>
-          </cell>
-          <cell r="L9">
-            <v>1366.7160706969223</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="F10">
-            <v>519.98804837156308</v>
-          </cell>
-          <cell r="H10">
-            <v>1149.5036363578847</v>
-          </cell>
-          <cell r="I10">
-            <v>403</v>
-          </cell>
-          <cell r="J10">
-            <v>533.331204843514</v>
-          </cell>
-          <cell r="L10">
-            <v>1358.3106030818005</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="F11">
-            <v>519.92902377304858</v>
-          </cell>
-          <cell r="H11">
-            <v>1141.9420694588671</v>
-          </cell>
-          <cell r="I11">
-            <v>404</v>
-          </cell>
-          <cell r="J11">
-            <v>533.2827969047953</v>
-          </cell>
-          <cell r="L11">
-            <v>1349.8968696318898</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="F12">
-            <v>519.86989943711774</v>
-          </cell>
-          <cell r="H12">
-            <v>1134.3699793277324</v>
-          </cell>
-          <cell r="I12">
-            <v>405</v>
-          </cell>
-          <cell r="J12">
-            <v>533.23430707610885</v>
-          </cell>
-          <cell r="L12">
-            <v>1341.4747148171773</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="F13">
-            <v>519.81067559905296</v>
-          </cell>
-          <cell r="H13">
-            <v>1126.787153813887</v>
-          </cell>
-          <cell r="I13">
-            <v>406</v>
-          </cell>
-          <cell r="J13">
-            <v>533.1857355501686</v>
-          </cell>
-          <cell r="L13">
-            <v>1333.0439790194471</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="F14">
-            <v>519.75135249379127</v>
-          </cell>
-          <cell r="H14">
-            <v>1119.1933747123417</v>
-          </cell>
-          <cell r="I14">
-            <v>407</v>
-          </cell>
-          <cell r="J14">
-            <v>533.13708251940807</v>
-          </cell>
-          <cell r="L14">
-            <v>1324.6044983920649</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="F15">
-            <v>519.69193035592275</v>
-          </cell>
-          <cell r="H15">
-            <v>1111.5884175359151</v>
-          </cell>
-          <cell r="I15">
-            <v>408</v>
-          </cell>
-          <cell r="J15">
-            <v>533.08834817597779</v>
-          </cell>
-          <cell r="L15">
-            <v>1316.1561047137641</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="F16">
-            <v>519.63240941968843</v>
-          </cell>
-          <cell r="H16">
-            <v>1103.9720512766617</v>
-          </cell>
-          <cell r="I16">
-            <v>409</v>
-          </cell>
-          <cell r="J16">
-            <v>533.03953271174476</v>
-          </cell>
-          <cell r="L16">
-            <v>1307.6986252361223</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="F17">
-            <v>519.57278991897897</v>
-          </cell>
-          <cell r="H17">
-            <v>1096.3440381559067</v>
-          </cell>
-          <cell r="I17">
-            <v>410</v>
-          </cell>
-          <cell r="J17">
-            <v>532.9906363182904</v>
-          </cell>
-          <cell r="L17">
-            <v>1299.231882524402</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="F18">
-            <v>519.51307208733249</v>
-          </cell>
-          <cell r="H18">
-            <v>1088.704133362228</v>
-          </cell>
-          <cell r="I18">
-            <v>411</v>
-          </cell>
-          <cell r="J18">
-            <v>532.94165918690953</v>
-          </cell>
-          <cell r="L18">
-            <v>1290.7556942914018</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="F19">
-            <v>519.45325615793377</v>
-          </cell>
-          <cell r="H19">
-            <v>1081.0520847766772</v>
-          </cell>
-          <cell r="I19">
-            <v>412</v>
-          </cell>
-          <cell r="J19">
-            <v>532.89260150860912</v>
-          </cell>
-          <cell r="L19">
-            <v>1282.2698732239551</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="F20">
-            <v>519.39334236361174</v>
-          </cell>
-          <cell r="H20">
-            <v>1073.3876326844836</v>
-          </cell>
-          <cell r="I20">
-            <v>413</v>
-          </cell>
-          <cell r="J20">
-            <v>532.84346347410644</v>
-          </cell>
-          <cell r="L20">
-            <v>1273.7742268016721</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="F21">
-            <v>519.33333093683825</v>
-          </cell>
-          <cell r="H21">
-            <v>1065.7105094724366</v>
-          </cell>
-          <cell r="I21">
-            <v>414</v>
-          </cell>
-          <cell r="J21">
-            <v>532.79424527382832</v>
-          </cell>
-          <cell r="L21">
-            <v>1265.2685571075172</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="F22">
-            <v>519.2732221097267</v>
-          </cell>
-          <cell r="H22">
-            <v>1058.0204393110748</v>
-          </cell>
-          <cell r="I22">
-            <v>415</v>
-          </cell>
-          <cell r="J22">
-            <v>532.7449470979094</v>
-          </cell>
-          <cell r="L22">
-            <v>1256.7526606297677</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="F23">
-            <v>519.21301611402998</v>
-          </cell>
-          <cell r="H23">
-            <v>1050.317137820763</v>
-          </cell>
-          <cell r="I23">
-            <v>416</v>
-          </cell>
-          <cell r="J23">
-            <v>532.69556913619101</v>
-          </cell>
-          <cell r="L23">
-            <v>1248.2263280548855</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="F24">
-            <v>519.15271318113935</v>
-          </cell>
-          <cell r="H24">
-            <v>1042.6003117206517</v>
-          </cell>
-          <cell r="I24">
-            <v>417</v>
-          </cell>
-          <cell r="J24">
-            <v>532.64611157822003</v>
-          </cell>
-          <cell r="L24">
-            <v>1239.6893440507934</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="F25">
-            <v>519.09231354208259</v>
-          </cell>
-          <cell r="H25">
-            <v>1034.8696584594602</v>
-          </cell>
-          <cell r="I25">
-            <v>418</v>
-          </cell>
-          <cell r="J25">
-            <v>532.59657461324741</v>
-          </cell>
-          <cell r="L25">
-            <v>1231.1414870400199</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="F26">
-            <v>519.03181742752281</v>
-          </cell>
-          <cell r="H26">
-            <v>1027.1248658269355</v>
-          </cell>
-          <cell r="I26">
-            <v>419</v>
-          </cell>
-          <cell r="J26">
-            <v>532.54695843022705</v>
-          </cell>
-          <cell r="L26">
-            <v>1222.582528962138</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="F27">
-            <v>518.97122506775668</v>
-          </cell>
-          <cell r="H27">
-            <v>1019.365611544749</v>
-          </cell>
-          <cell r="I27">
-            <v>420</v>
-          </cell>
-          <cell r="J27">
-            <v>532.49726321781452</v>
-          </cell>
-          <cell r="L27">
-            <v>1214.0122350248878</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="F28">
-            <v>518.91053669271332</v>
-          </cell>
-          <cell r="H28">
-            <v>1011.5915628355151</v>
-          </cell>
-          <cell r="I28">
-            <v>421</v>
-          </cell>
-          <cell r="J28">
-            <v>532.44748916436606</v>
-          </cell>
-          <cell r="L28">
-            <v>1205.430363443327</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="F29">
-            <v>518.84975253195239</v>
-          </cell>
-          <cell r="H29">
-            <v>1003.8023759684971</v>
-          </cell>
-          <cell r="I29">
-            <v>422</v>
-          </cell>
-          <cell r="J29">
-            <v>532.39763645793687</v>
-          </cell>
-          <cell r="L29">
-            <v>1196.8366651663123</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="F30">
-            <v>518.78887281466314</v>
-          </cell>
-          <cell r="H30">
-            <v>995.99769578046721</v>
-          </cell>
-          <cell r="I30">
-            <v>423</v>
-          </cell>
-          <cell r="J30">
-            <v>532.34770528628076</v>
-          </cell>
-          <cell r="L30">
-            <v>1188.2308835895697</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="F31">
-            <v>518.7278977696626</v>
-          </cell>
-          <cell r="H31">
-            <v>988.17715517006366</v>
-          </cell>
-          <cell r="I31">
-            <v>424</v>
-          </cell>
-          <cell r="J31">
-            <v>532.29769583684811</v>
-          </cell>
-          <cell r="L31">
-            <v>1179.6127542545478</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="F32">
-            <v>518.66682762539449</v>
-          </cell>
-          <cell r="H32">
-            <v>980.34037456385522</v>
-          </cell>
-          <cell r="I32">
-            <v>425</v>
-          </cell>
-          <cell r="J32">
-            <v>532.2476082967853</v>
-          </cell>
-          <cell r="L32">
-            <v>1170.9820045322094</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="F33">
-            <v>518.60566260992778</v>
-          </cell>
-          <cell r="H33">
-            <v>972.48696135218188</v>
-          </cell>
-          <cell r="I33">
-            <v>426</v>
-          </cell>
-          <cell r="J33">
-            <v>532.1974428529337</v>
-          </cell>
-          <cell r="L33">
-            <v>1162.3383532908413</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="F34">
-            <v>518.54440295095537</v>
-          </cell>
-          <cell r="H34">
-            <v>964.61650929268262</v>
-          </cell>
-          <cell r="I34">
-            <v>427</v>
-          </cell>
-          <cell r="J34">
-            <v>532.14719969182795</v>
-          </cell>
-          <cell r="L34">
-            <v>1153.6815105469004</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="F35">
-            <v>518.48304887579286</v>
-          </cell>
-          <cell r="H35">
-            <v>956.72859787925222</v>
-          </cell>
-          <cell r="I35">
-            <v>428</v>
-          </cell>
-          <cell r="J35">
-            <v>532.09687899969549</v>
-          </cell>
-          <cell r="L35">
-            <v>1145.0111770978535</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="F36">
-            <v>518.42160061137679</v>
-          </cell>
-          <cell r="H36">
-            <v>948.82279167397746</v>
-          </cell>
-          <cell r="I36">
-            <v>429</v>
-          </cell>
-          <cell r="J36">
-            <v>532.04648096245512</v>
-          </cell>
-          <cell r="L36">
-            <v>1136.327044135872</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="F37">
-            <v>518.36005838426411</v>
-          </cell>
-          <cell r="H37">
-            <v>940.89863959939919</v>
-          </cell>
-          <cell r="I37">
-            <v>430</v>
-          </cell>
-          <cell r="J37">
-            <v>531.99600576571606</v>
-          </cell>
-          <cell r="L37">
-            <v>1127.6287928411746</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="F38">
-            <v>518.29842242063023</v>
-          </cell>
-          <cell r="H38">
-            <v>932.95567418822202</v>
-          </cell>
-          <cell r="I38">
-            <v>431</v>
-          </cell>
-          <cell r="J38">
-            <v>531.94545359477695</v>
-          </cell>
-          <cell r="L38">
-            <v>1118.9160939537164</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="F39">
-            <v>518.23669294626836</v>
-          </cell>
-          <cell r="H39">
-            <v>924.99341078734176</v>
-          </cell>
-          <cell r="I39">
-            <v>432</v>
-          </cell>
-          <cell r="J39">
-            <v>531.89482463462491</v>
-          </cell>
-          <cell r="L39">
-            <v>1110.1886073218193</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="F40">
-            <v>518.17487018658767</v>
-          </cell>
-          <cell r="H40">
-            <v>917.01134671278749</v>
-          </cell>
-          <cell r="I40">
-            <v>433</v>
-          </cell>
-          <cell r="J40">
-            <v>531.84411906993432</v>
-          </cell>
-          <cell r="L40">
-            <v>1101.4459814262341</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="F41">
-            <v>518.11295436661294</v>
-          </cell>
-          <cell r="H41">
-            <v>909.00896035187691</v>
-          </cell>
-          <cell r="I41">
-            <v>434</v>
-          </cell>
-          <cell r="J41">
-            <v>531.7933370850659</v>
-          </cell>
-          <cell r="L41">
-            <v>1092.6878528780121</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="F42">
-            <v>518.05094571098232</v>
-          </cell>
-          <cell r="H42">
-            <v>900.98571020854706</v>
-          </cell>
-          <cell r="I42">
-            <v>435</v>
-          </cell>
-          <cell r="J42">
-            <v>531.74247886406579</v>
-          </cell>
-          <cell r="L42">
-            <v>1083.9138458884277</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="F43">
-            <v>517.98884444394707</v>
-          </cell>
-          <cell r="H43">
-            <v>892.94103388745657</v>
-          </cell>
-          <cell r="I43">
-            <v>436</v>
-          </cell>
-          <cell r="J43">
-            <v>531.69154459066476</v>
-          </cell>
-          <cell r="L43">
-            <v>1075.1235717090592</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="F44">
-            <v>517.92665078937</v>
-          </cell>
-          <cell r="H44">
-            <v>884.87434701204893</v>
-          </cell>
-          <cell r="I44">
-            <v>437</v>
-          </cell>
-          <cell r="J44">
-            <v>531.64053444827675</v>
-          </cell>
-          <cell r="L44">
-            <v>1066.3166280399871</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="F45">
-            <v>517.86436497072441</v>
-          </cell>
-          <cell r="H45">
-            <v>876.78504207131641</v>
-          </cell>
-          <cell r="I45">
-            <v>438</v>
-          </cell>
-          <cell r="J45">
-            <v>531.58944861999862</v>
-          </cell>
-          <cell r="L45">
-            <v>1057.4925984038907</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="F46">
-            <v>517.80198721109309</v>
-          </cell>
-          <cell r="H46">
-            <v>868.67248718950464</v>
-          </cell>
-          <cell r="I46">
-            <v>439</v>
-          </cell>
-          <cell r="J46">
-            <v>531.53828728860879</v>
-          </cell>
-          <cell r="L46">
-            <v>1048.6510514836561</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="F47">
-            <v>517.73951773316708</v>
-          </cell>
-          <cell r="H47">
-            <v>860.53602481244207</v>
-          </cell>
-          <cell r="I47">
-            <v>440</v>
-          </cell>
-          <cell r="J47">
-            <v>531.48705063656621</v>
-          </cell>
-          <cell r="L47">
-            <v>1039.7915404208982</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="F48">
-            <v>517.6769567592446</v>
-          </cell>
-          <cell r="H48">
-            <v>852.37497030356303</v>
-          </cell>
-          <cell r="I48">
-            <v>441</v>
-          </cell>
-          <cell r="J48">
-            <v>531.43573884601005</v>
-          </cell>
-          <cell r="L48">
-            <v>1030.9136020725848</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="F49">
-            <v>517.61430451123033</v>
-          </cell>
-          <cell r="H49">
-            <v>844.1886104420031</v>
-          </cell>
-          <cell r="I49">
-            <v>442</v>
-          </cell>
-          <cell r="J49">
-            <v>531.38435209875843</v>
-          </cell>
-          <cell r="L49">
-            <v>1022.0167562227148</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="F50">
-            <v>517.55156121063396</v>
-          </cell>
-          <cell r="H50">
-            <v>835.97620181438174</v>
-          </cell>
-          <cell r="I50">
-            <v>443</v>
-          </cell>
-          <cell r="J50">
-            <v>531.33289057630759</v>
-          </cell>
-          <cell r="L50">
-            <v>1013.1005047457282</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="F51">
-            <v>517.48872707856913</v>
-          </cell>
-          <cell r="H51">
-            <v>827.73696909102716</v>
-          </cell>
-          <cell r="I51">
-            <v>444</v>
-          </cell>
-          <cell r="J51">
-            <v>531.28135445983116</v>
-          </cell>
-          <cell r="L51">
-            <v>1004.1643307180452</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="F52">
-            <v>517.42580233575325</v>
-          </cell>
-          <cell r="H52">
-            <v>819.47010317643685</v>
-          </cell>
-          <cell r="I52">
-            <v>445</v>
-          </cell>
-          <cell r="J52">
-            <v>531.2297439301791</v>
-          </cell>
-          <cell r="L52">
-            <v>995.20769747380427</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="F53">
-            <v>517.36278720250527</v>
-          </cell>
-          <cell r="H53">
-            <v>811.17475922269671</v>
-          </cell>
-          <cell r="I53">
-            <v>446</v>
-          </cell>
-          <cell r="J53">
-            <v>531.17805916787745</v>
-          </cell>
-          <cell r="L53">
-            <v>986.2300476005197</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="F54">
-            <v>517.29968189874603</v>
-          </cell>
-          <cell r="H54">
-            <v>802.85005449336563</v>
-          </cell>
-          <cell r="I54">
-            <v>447</v>
-          </cell>
-          <cell r="J54">
-            <v>531.12630035312702</v>
-          </cell>
-          <cell r="L54">
-            <v>977.23080186998652</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="F55">
-            <v>517.23648664399616</v>
-          </cell>
-          <cell r="H55">
-            <v>794.49506606397506</v>
-          </cell>
-          <cell r="I55">
-            <v>448</v>
-          </cell>
-          <cell r="J55">
-            <v>531.07446766580256</v>
-          </cell>
-          <cell r="L55">
-            <v>968.20935809932712</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="F56">
-            <v>517.17320165737601</v>
-          </cell>
-          <cell r="H56">
-            <v>786.10882834376059</v>
-          </cell>
-          <cell r="I56">
-            <v>449</v>
-          </cell>
-          <cell r="J56">
-            <v>531.02256128545253</v>
-          </cell>
-          <cell r="L56">
-            <v>959.16508993660022</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="F57">
-            <v>517.10982715760429</v>
-          </cell>
-          <cell r="H57">
-            <v>777.69033040150373</v>
-          </cell>
-          <cell r="I57">
-            <v>450</v>
-          </cell>
-          <cell r="J57">
-            <v>530.97058139129774</v>
-          </cell>
-          <cell r="L57">
-            <v>950.09734556485455</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="F58">
-            <v>517.04636336299734</v>
-          </cell>
-          <cell r="H58">
-            <v>769.23851307640609</v>
-          </cell>
-          <cell r="I58">
-            <v>451</v>
-          </cell>
-          <cell r="J58">
-            <v>530.91852816223138</v>
-          </cell>
-          <cell r="L58">
-            <v>941.0054463179265</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="F59">
-            <v>516.98281049146829</v>
-          </cell>
-          <cell r="H59">
-            <v>760.75226585268877</v>
-          </cell>
-          <cell r="I59">
-            <v>452</v>
-          </cell>
-          <cell r="J59">
-            <v>530.86640177681727</v>
-          </cell>
-          <cell r="L59">
-            <v>931.88868520061897</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="F60">
-            <v>516.91916876052608</v>
-          </cell>
-          <cell r="H60">
-            <v>752.2304234740842</v>
-          </cell>
-          <cell r="I60">
-            <v>453</v>
-          </cell>
-          <cell r="J60">
-            <v>530.81420241328999</v>
-          </cell>
-          <cell r="L60">
-            <v>922.74632530517158</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="F61">
-            <v>516.85543838727472</v>
-          </cell>
-          <cell r="H61">
-            <v>743.67176227150105</v>
-          </cell>
-          <cell r="I61">
-            <v>454</v>
-          </cell>
-          <cell r="J61">
-            <v>530.7619302495541</v>
-          </cell>
-          <cell r="L61">
-            <v>913.57759811511232</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="F62">
-            <v>516.79161958841269</v>
-          </cell>
-          <cell r="H62">
-            <v>735.07499617385974</v>
-          </cell>
-          <cell r="I62">
-            <v>455</v>
-          </cell>
-          <cell r="J62">
-            <v>530.70958546318286</v>
-          </cell>
-          <cell r="L62">
-            <v>904.38170168667114</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="F63">
-            <v>516.72771258023158</v>
-          </cell>
-          <cell r="H63">
-            <v>726.43877236832566</v>
-          </cell>
-          <cell r="I63">
-            <v>456</v>
-          </cell>
-          <cell r="J63">
-            <v>530.65716823141838</v>
-          </cell>
-          <cell r="L63">
-            <v>895.15779869691198</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="F64">
-            <v>516.66371757861566</v>
-          </cell>
-          <cell r="H64">
-            <v>717.76166657185024</v>
-          </cell>
-          <cell r="I64">
-            <v>457</v>
-          </cell>
-          <cell r="J64">
-            <v>530.60467873117034</v>
-          </cell>
-          <cell r="L64">
-            <v>885.90501434659711</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="F65">
-            <v>516.5996347990415</v>
-          </cell>
-          <cell r="H65">
-            <v>709.04217787096411</v>
-          </cell>
-          <cell r="I65">
-            <v>458</v>
-          </cell>
-          <cell r="J65">
-            <v>530.55211713901565</v>
-          </cell>
-          <cell r="L65">
-            <v>876.62243410450583</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="F66">
-            <v>516.53546445657639</v>
-          </cell>
-          <cell r="H66">
-            <v>700.27872308103156</v>
-          </cell>
-          <cell r="I66">
-            <v>459</v>
-          </cell>
-          <cell r="J66">
-            <v>530.4994836311979</v>
-          </cell>
-          <cell r="L66">
-            <v>867.30910127848529</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="F67">
-            <v>516.47120676587826</v>
-          </cell>
-          <cell r="H67">
-            <v>691.46963056955735</v>
-          </cell>
-          <cell r="I67">
-            <v>460</v>
-          </cell>
-          <cell r="J67">
-            <v>530.44677838362645</v>
-          </cell>
-          <cell r="L67">
-            <v>857.9640143968744</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="F68">
-            <v>516.40686194119451</v>
-          </cell>
-          <cell r="H68">
-            <v>682.61313348045098</v>
-          </cell>
-          <cell r="I68">
-            <v>461</v>
-          </cell>
-          <cell r="J68">
-            <v>530.39400157187617</v>
-          </cell>
-          <cell r="L68">
-            <v>848.58612438209661</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="F69">
-            <v>516.34243019636176</v>
-          </cell>
-          <cell r="H69">
-            <v>673.70736228721739</v>
-          </cell>
-          <cell r="I69">
-            <v>462</v>
-          </cell>
-          <cell r="J69">
-            <v>530.34115337118658</v>
-          </cell>
-          <cell r="L69">
-            <v>839.17433149612918</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="F70">
-            <v>516.2779117448049</v>
-          </cell>
-          <cell r="H70">
-            <v>664.75033659261874</v>
-          </cell>
-          <cell r="I70">
-            <v>463</v>
-          </cell>
-          <cell r="J70">
-            <v>530.28823395646134</v>
-          </cell>
-          <cell r="L70">
-            <v>829.72748203518267</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="F71">
-            <v>516.21330679953644</v>
-          </cell>
-          <cell r="H71">
-            <v>655.73995608015218</v>
-          </cell>
-          <cell r="I71">
-            <v>464</v>
-          </cell>
-          <cell r="J71">
-            <v>530.23524350226796</v>
-          </cell>
-          <cell r="L71">
-            <v>820.24436474823437</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="F72">
-            <v>516.14861557315578</v>
-          </cell>
-          <cell r="H72">
-            <v>646.6739905083549</v>
-          </cell>
-          <cell r="I72">
-            <v>465</v>
-          </cell>
-          <cell r="J72">
-            <v>530.18218218283687</v>
-          </cell>
-          <cell r="L72">
-            <v>810.72370695098436</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="F73">
-            <v>516.08383827784894</v>
-          </cell>
-          <cell r="H73">
-            <v>637.55006862206517</v>
-          </cell>
-          <cell r="I73">
-            <v>466</v>
-          </cell>
-          <cell r="J73">
-            <v>530.12905017206128</v>
-          </cell>
-          <cell r="L73">
-            <v>801.16417030330172</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="F74">
-            <v>516.01897512538733</v>
-          </cell>
-          <cell r="H74">
-            <v>628.36566583479078</v>
-          </cell>
-          <cell r="I74">
-            <v>467</v>
-          </cell>
-          <cell r="J74">
-            <v>530.0758476434961</v>
-          </cell>
-          <cell r="L74">
-            <v>791.56434621421067</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="F75">
-            <v>515.95402632712774</v>
-          </cell>
-          <cell r="H75">
-            <v>619.11809051262583</v>
-          </cell>
-          <cell r="I75">
-            <v>468</v>
-          </cell>
-          <cell r="J75">
-            <v>530.02257477035823</v>
-          </cell>
-          <cell r="L75">
-            <v>781.92275083386915</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="F76">
-            <v>515.88899209401143</v>
-          </cell>
-          <cell r="H76">
-            <v>609.80446866188174</v>
-          </cell>
-          <cell r="I76">
-            <v>469</v>
-          </cell>
-          <cell r="J76">
-            <v>529.96923172552533</v>
-          </cell>
-          <cell r="L76">
-            <v>772.23781958668656</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="F77">
-            <v>515.82387263656358</v>
-          </cell>
-          <cell r="H77">
-            <v>600.42172678876307</v>
-          </cell>
-          <cell r="I77">
-            <v>470</v>
-          </cell>
-          <cell r="J77">
-            <v>529.91581868153571</v>
-          </cell>
-          <cell r="L77">
-            <v>762.50790119363091</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="F78">
-            <v>515.75866816489281</v>
-          </cell>
-          <cell r="H78">
-            <v>590.96657265872489</v>
-          </cell>
-          <cell r="I78">
-            <v>471</v>
-          </cell>
-          <cell r="J78">
-            <v>529.86233581058787</v>
-          </cell>
-          <cell r="L78">
-            <v>752.73125112469802</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="F79">
-            <v>515.69337888869063</v>
-          </cell>
-          <cell r="H79">
-            <v>581.43547363400523</v>
-          </cell>
-          <cell r="I79">
-            <v>472</v>
-          </cell>
-          <cell r="J79">
-            <v>529.80878328453969</v>
-          </cell>
-          <cell r="L79">
-            <v>742.90602441433407</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="F80">
-            <v>515.62800501723086</v>
-          </cell>
-          <cell r="H80">
-            <v>571.82463220816226</v>
-          </cell>
-          <cell r="I80">
-            <v>473</v>
-          </cell>
-          <cell r="J80">
-            <v>529.7551612749088</v>
-          </cell>
-          <cell r="L80">
-            <v>733.03026776306456</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="F81">
-            <v>515.56254675936907</v>
-          </cell>
-          <cell r="H81">
-            <v>562.12995828366945</v>
-          </cell>
-          <cell r="I81">
-            <v>474</v>
-          </cell>
-          <cell r="J81">
-            <v>529.70146995287109</v>
-          </cell>
-          <cell r="L81">
-            <v>723.10191083746281</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="F82">
-            <v>515.49700432354223</v>
-          </cell>
-          <cell r="H82">
-            <v>552.34703764933863</v>
-          </cell>
-          <cell r="I82">
-            <v>475</v>
-          </cell>
-          <cell r="J82">
-            <v>529.64770948926116</v>
-          </cell>
-          <cell r="L82">
-            <v>713.11875666757714</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="F83">
-            <v>515.43137791776803</v>
-          </cell>
-          <cell r="H83">
-            <v>542.47109600420185</v>
-          </cell>
-          <cell r="I83">
-            <v>476</v>
-          </cell>
-          <cell r="J83">
-            <v>529.5938800545714</v>
-          </cell>
-          <cell r="L83">
-            <v>703.07847102564097</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="F84">
-            <v>515.36566774964467</v>
-          </cell>
-          <cell r="H84">
-            <v>532.49695773778831</v>
-          </cell>
-          <cell r="I84">
-            <v>477</v>
-          </cell>
-          <cell r="J84">
-            <v>529.53998181895179</v>
-          </cell>
-          <cell r="L84">
-            <v>692.9785706518752</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="F85">
-            <v>515.29987402635015</v>
-          </cell>
-          <cell r="H85">
-            <v>522.4189985059885</v>
-          </cell>
-          <cell r="I85">
-            <v>478</v>
-          </cell>
-          <cell r="J85">
-            <v>529.48601495220964</v>
-          </cell>
-          <cell r="L85">
-            <v>682.81641017187042</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="F86">
-            <v>515.24869475196908</v>
-          </cell>
-          <cell r="H86">
-            <v>514.51285346428438</v>
-          </cell>
-          <cell r="I86">
-            <v>478.77699999999999</v>
-          </cell>
-          <cell r="J86">
-            <v>529.44403542456803</v>
-          </cell>
-          <cell r="L86">
-            <v>674.8756326036015</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="F87">
-            <v>515.18275306101248</v>
-          </cell>
-          <cell r="H87">
-            <v>504.2349247523025</v>
-          </cell>
-          <cell r="I87">
-            <v>479.77699999999999</v>
-          </cell>
-          <cell r="J87">
-            <v>529.38994701823083</v>
-          </cell>
-          <cell r="L87">
-            <v>664.59575018286387</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="F88">
-            <v>515.1167283880111</v>
-          </cell>
-          <cell r="H88">
-            <v>493.83471151789257</v>
-          </cell>
-          <cell r="I88">
-            <v>480.77699999999999</v>
-          </cell>
-          <cell r="J88">
-            <v>529.33579045052466</v>
-          </cell>
-          <cell r="L88">
-            <v>654.24528312740392</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="F89">
-            <v>515.0506209385527</v>
-          </cell>
-          <cell r="H89">
-            <v>483.30431951303746</v>
-          </cell>
-          <cell r="I89">
-            <v>481.77699999999999</v>
-          </cell>
-          <cell r="J89">
-            <v>529.28156588995887</v>
-          </cell>
-          <cell r="L89">
-            <v>643.8208271577671</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="F90">
-            <v>514.98443091780234</v>
-          </cell>
-          <cell r="H90">
-            <v>472.63504760011199</v>
-          </cell>
-          <cell r="I90">
-            <v>482.77699999999999</v>
-          </cell>
-          <cell r="J90">
-            <v>529.22727350469791</v>
-          </cell>
-          <cell r="L90">
-            <v>633.31872870150187</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="F91">
-            <v>514.91815853050298</v>
-          </cell>
-          <cell r="H91">
-            <v>461.81727033531365</v>
-          </cell>
-          <cell r="I91">
-            <v>483.77699999999999</v>
-          </cell>
-          <cell r="J91">
-            <v>529.17291346256161</v>
-          </cell>
-          <cell r="L91">
-            <v>622.73505957219322</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="F92">
-            <v>514.85180398097475</v>
-          </cell>
-          <cell r="H92">
-            <v>450.84029782170114</v>
-          </cell>
-          <cell r="I92">
-            <v>484.77699999999999</v>
-          </cell>
-          <cell r="J92">
-            <v>529.11848593102491</v>
-          </cell>
-          <cell r="L92">
-            <v>612.06558829181063</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="F93">
-            <v>514.78536747311443</v>
-          </cell>
-          <cell r="H93">
-            <v>439.69220723133151</v>
-          </cell>
-          <cell r="I93">
-            <v>485.77699999999999</v>
-          </cell>
-          <cell r="J93">
-            <v>529.06399107721722</v>
-          </cell>
-          <cell r="L93">
-            <v>601.30574749950506</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="F94">
-            <v>514.71884921039555</v>
-          </cell>
-          <cell r="H94">
-            <v>428.35963869155574</v>
-          </cell>
-          <cell r="I94">
-            <v>486.77699999999999</v>
-          </cell>
-          <cell r="J94">
-            <v>529.00942906792204</v>
-          </cell>
-          <cell r="L94">
-            <v>590.45059677774714</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="F95">
-            <v>514.65224939586733</v>
-          </cell>
-          <cell r="H95">
-            <v>416.82754589873281</v>
-          </cell>
-          <cell r="I95">
-            <v>487.77699999999999</v>
-          </cell>
-          <cell r="J95">
-            <v>528.95480006957735</v>
-          </cell>
-          <cell r="L95">
-            <v>579.49478008760184</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="F96">
-            <v>514.58556823215554</v>
-          </cell>
-          <cell r="H96">
-            <v>405.07888858833422</v>
-          </cell>
-          <cell r="I96">
-            <v>488.77699999999999</v>
-          </cell>
-          <cell r="J96">
-            <v>528.90010424827449</v>
-          </cell>
-          <cell r="L96">
-            <v>568.43247683139919</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="F97">
-            <v>514.51880592146085</v>
-          </cell>
-          <cell r="H97">
-            <v>393.09424943639169</v>
-          </cell>
-          <cell r="I97">
-            <v>489.77699999999999</v>
-          </cell>
-          <cell r="J97">
-            <v>528.84534176975876</v>
-          </cell>
-          <cell r="L97">
-            <v>557.25734534315598</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="F98">
-            <v>514.45196266555968</v>
-          </cell>
-          <cell r="H98">
-            <v>380.85135144825216</v>
-          </cell>
-          <cell r="I98">
-            <v>490.77699999999999</v>
-          </cell>
-          <cell r="J98">
-            <v>528.79051279942837</v>
-          </cell>
-          <cell r="L98">
-            <v>545.9624573314951</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="F99">
-            <v>514.38503866580311</v>
-          </cell>
-          <cell r="H99">
-            <v>368.32444238736053</v>
-          </cell>
-          <cell r="I99">
-            <v>491.77699999999999</v>
-          </cell>
-          <cell r="J99">
-            <v>528.73561750233489</v>
-          </cell>
-          <cell r="L99">
-            <v>534.54022144859107</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="F100">
-            <v>514.31803412311729</v>
-          </cell>
-          <cell r="H100">
-            <v>355.48349866057094</v>
-          </cell>
-          <cell r="I100">
-            <v>492.77699999999999</v>
-          </cell>
-          <cell r="J100">
-            <v>528.68065604318247</v>
-          </cell>
-          <cell r="L100">
-            <v>522.982293707439</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="F101">
-            <v>514.2509492380027</v>
-          </cell>
-          <cell r="H101">
-            <v>342.29317956973682</v>
-          </cell>
-          <cell r="I101">
-            <v>493.77699999999999</v>
-          </cell>
-          <cell r="J101">
-            <v>528.62562858632839</v>
-          </cell>
-          <cell r="L101">
-            <v>511.27947188499576</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="F102">
-            <v>514.18378421053421</v>
-          </cell>
-          <cell r="H102">
-            <v>328.7114292810034</v>
-          </cell>
-          <cell r="I102">
-            <v>494.77699999999999</v>
-          </cell>
-          <cell r="J102">
-            <v>528.57053529578172</v>
-          </cell>
-          <cell r="L102">
-            <v>499.42157028389079</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="F103">
-            <v>514.11653924036045</v>
-          </cell>
-          <cell r="H103">
-            <v>314.68756998006785</v>
-          </cell>
-          <cell r="I103">
-            <v>495.77699999999999</v>
-          </cell>
-          <cell r="J103">
-            <v>528.51537633520434</v>
-          </cell>
-          <cell r="L103">
-            <v>487.39727021494019</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="F104">
-            <v>514.04921452670442</v>
-          </cell>
-          <cell r="H104">
-            <v>300.15964029156237</v>
-          </cell>
-          <cell r="I104">
-            <v>496.77699999999999</v>
-          </cell>
-          <cell r="J104">
-            <v>528.46015186790987</v>
-          </cell>
-          <cell r="L104">
-            <v>475.19394021330345</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="F105">
-            <v>513.98181026836221</v>
-          </cell>
-          <cell r="H105">
-            <v>285.05057905564775</v>
-          </cell>
-          <cell r="I105">
-            <v>497.77699999999999</v>
-          </cell>
-          <cell r="J105">
-            <v>528.40486205686409</v>
-          </cell>
-          <cell r="L105">
-            <v>462.79741817801312</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="F106">
-            <v>513.91432666370383</v>
-          </cell>
-          <cell r="H106">
-            <v>269.26257738490159</v>
-          </cell>
-          <cell r="I106">
-            <v>498.77699999999999</v>
-          </cell>
-          <cell r="J106">
-            <v>528.3495070646843</v>
-          </cell>
-          <cell r="L106">
-            <v>450.19174513016765</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="F107">
-            <v>513.84676391067239</v>
-          </cell>
-          <cell r="H107">
-            <v>252.66839640121222</v>
-          </cell>
-          <cell r="I107">
-            <v>499.77699999999999</v>
-          </cell>
-          <cell r="J107">
-            <v>528.29408705363971</v>
-          </cell>
-          <cell r="L107">
-            <v>437.35883682484109</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="F108">
-            <v>513.77912220678411</v>
-          </cell>
-          <cell r="H108">
-            <v>235.09738726740486</v>
-          </cell>
-          <cell r="I108">
-            <v>500.77699999999999</v>
-          </cell>
-          <cell r="J108">
-            <v>528.23860218565051</v>
-          </cell>
-          <cell r="L108">
-            <v>424.2780745790796</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="F109">
-            <v>513.71140174912841</v>
-          </cell>
-          <cell r="H109">
-            <v>216.31163736600061</v>
-          </cell>
-          <cell r="I109">
-            <v>501.77699999999999</v>
-          </cell>
-          <cell r="J109">
-            <v>528.18305262228887</v>
-          </cell>
-          <cell r="L109">
-            <v>410.92578970247797</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="F110">
-            <v>513.64360273436716</v>
-          </cell>
-          <cell r="H110">
-            <v>195.96210710226651</v>
-          </cell>
-          <cell r="I110">
-            <v>502.77699999999999</v>
-          </cell>
-          <cell r="J110">
-            <v>528.12743852477763</v>
-          </cell>
-          <cell r="L110">
-            <v>397.27460574645363</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="F111">
-            <v>513.57572535873555</v>
-          </cell>
-          <cell r="H111">
-            <v>173.49942472515616</v>
-          </cell>
-          <cell r="I111">
-            <v>503.77699999999999</v>
-          </cell>
-          <cell r="J111">
-            <v>528.07176005399094</v>
-          </cell>
-          <cell r="L111">
-            <v>383.29258765819651</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="F112">
-            <v>513.50776981804097</v>
-          </cell>
-          <cell r="H112">
-            <v>147.96429751788125</v>
-          </cell>
-          <cell r="I112">
-            <v>504.77699999999999</v>
-          </cell>
-          <cell r="J112">
-            <v>528.01601737045416</v>
-          </cell>
-          <cell r="L112">
-            <v>368.94212390394415</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="F113">
-            <v>513.43973630766334</v>
-          </cell>
-          <cell r="H113">
-            <v>117.36820821653585</v>
-          </cell>
-          <cell r="I113">
-            <v>505.77699999999999</v>
-          </cell>
-          <cell r="J113">
-            <v>527.9602106343433</v>
-          </cell>
-          <cell r="L113">
-            <v>354.17843170090305</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="F114">
-            <v>513.37162502255524</v>
-          </cell>
-          <cell r="H114">
-            <v>75.813186583602672</v>
-          </cell>
-          <cell r="I114">
-            <v>506.77699999999999</v>
-          </cell>
-          <cell r="J114">
-            <v>527.90434000548544</v>
-          </cell>
-          <cell r="L114">
-            <v>338.94751780738903</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="F115">
-            <v>513.30343615724166</v>
-          </cell>
-          <cell r="H115" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I115">
-            <v>507.77699999999999</v>
-          </cell>
-          <cell r="J115">
-            <v>527.84840564335809</v>
-          </cell>
-          <cell r="L115">
-            <v>323.18333160574713</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="F116">
-            <v>513.23516990581948</v>
-          </cell>
-          <cell r="H116" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I116">
-            <v>508.77699999999999</v>
-          </cell>
-          <cell r="J116">
-            <v>527.79240770708986</v>
-          </cell>
-          <cell r="L116">
-            <v>306.80368231511051</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="F117">
-            <v>513.16682646195807</v>
-          </cell>
-          <cell r="H117" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I117">
-            <v>509.77699999999999</v>
-          </cell>
-          <cell r="J117">
-            <v>527.73634635545977</v>
-          </cell>
-          <cell r="L117">
-            <v>289.70419532818846</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="F118">
-            <v>513.09840601889914</v>
-          </cell>
-          <cell r="H118" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I118">
-            <v>510.77699999999999</v>
-          </cell>
-          <cell r="J118">
-            <v>527.68022174689759</v>
-          </cell>
-          <cell r="L118">
-            <v>271.74901978427846</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="F119">
-            <v>513.02990876945637</v>
-          </cell>
-          <cell r="H119" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I119">
-            <v>511.77699999999999</v>
-          </cell>
-          <cell r="J119">
-            <v>527.6240340394836</v>
-          </cell>
-          <cell r="L119">
-            <v>252.75586317828538</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="F120">
-            <v>512.96133490601551</v>
-          </cell>
-          <cell r="H120" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I120">
-            <v>512.77700000000004</v>
-          </cell>
-          <cell r="J120">
-            <v>527.56778339094853</v>
-          </cell>
-          <cell r="L120">
-            <v>232.47045111713561</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="F121">
-            <v>512.89268462053462</v>
-          </cell>
-          <cell r="H121" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I121">
-            <v>513.77700000000004</v>
-          </cell>
-          <cell r="J121">
-            <v>527.51146995867384</v>
-          </cell>
-          <cell r="L121">
-            <v>210.5195538864038</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="F122">
-            <v>512.82395810454375</v>
-          </cell>
-          <cell r="H122" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I122">
-            <v>514.77700000000004</v>
-          </cell>
-          <cell r="J122">
-            <v>527.45509389969141</v>
-          </cell>
-          <cell r="L122">
-            <v>186.31543722616598</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="F123">
-            <v>512.75515554914512</v>
-          </cell>
-          <cell r="H123" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I123">
-            <v>515.77700000000004</v>
-          </cell>
-          <cell r="J123">
-            <v>527.39865537068351</v>
-          </cell>
-          <cell r="L123">
-            <v>158.83132368442094</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="F124">
-            <v>512.68627714501304</v>
-          </cell>
-          <cell r="H124" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I124">
-            <v>516.77700000000004</v>
-          </cell>
-          <cell r="J124">
-            <v>527.34215452798321</v>
-          </cell>
-          <cell r="L124">
-            <v>125.93777936836186</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="F125">
-            <v>512.61732308239414</v>
-          </cell>
-          <cell r="H125" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I125">
-            <v>517.77700000000004</v>
-          </cell>
-          <cell r="J125">
-            <v>527.28559152757396</v>
-          </cell>
-          <cell r="L125">
-            <v>81.315723051843207</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="F126">
-            <v>512.54829355110712</v>
-          </cell>
-          <cell r="H126" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I126">
-            <v>518.77700000000004</v>
-          </cell>
-          <cell r="J126">
-            <v>527.22896652508973</v>
-          </cell>
-          <cell r="L126" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="F127">
-            <v>512.47918874054312</v>
-          </cell>
-          <cell r="H127" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I127">
-            <v>519.77700000000004</v>
-          </cell>
-          <cell r="J127">
-            <v>527.17227967581528</v>
-          </cell>
-          <cell r="L127" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="F128">
-            <v>512.41000883966524</v>
-          </cell>
-          <cell r="H128" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I128">
-            <v>520.77700000000004</v>
-          </cell>
-          <cell r="J128">
-            <v>527.11553113468574</v>
-          </cell>
-          <cell r="L128" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="F129">
-            <v>512.34075403700945</v>
-          </cell>
-          <cell r="H129" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I129">
-            <v>521.77700000000004</v>
-          </cell>
-          <cell r="J129">
-            <v>527.05872105628714</v>
-          </cell>
-          <cell r="L129" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="F130">
-            <v>512.27142452068369</v>
-          </cell>
-          <cell r="H130" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I130">
-            <v>522.77700000000004</v>
-          </cell>
-          <cell r="J130">
-            <v>527.00184959485614</v>
-          </cell>
-          <cell r="L130" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="F131">
-            <v>512.20202047836904</v>
-          </cell>
-          <cell r="H131" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I131">
-            <v>523.77700000000004</v>
-          </cell>
-          <cell r="J131">
-            <v>526.94491690428038</v>
-          </cell>
-          <cell r="L131" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="F132">
-            <v>512.13254209731872</v>
-          </cell>
-          <cell r="H132" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I132">
-            <v>524.77700000000004</v>
-          </cell>
-          <cell r="J132">
-            <v>526.88792313809824</v>
-          </cell>
-          <cell r="L132" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="F133">
-            <v>512.06298956435887</v>
-          </cell>
-          <cell r="H133" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I133">
-            <v>525.77700000000004</v>
-          </cell>
-          <cell r="J133">
-            <v>526.83086844949901</v>
-          </cell>
-          <cell r="L133" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="F134">
-            <v>511.99336306588867</v>
-          </cell>
-          <cell r="H134" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I134">
-            <v>526.77700000000004</v>
-          </cell>
-          <cell r="J134">
-            <v>526.77375299132314</v>
-          </cell>
-          <cell r="L134" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="F135">
-            <v>511.92366278788018</v>
-          </cell>
-          <cell r="H135" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I135">
-            <v>527.77700000000004</v>
-          </cell>
-          <cell r="J135">
-            <v>526.71657691606231</v>
-          </cell>
-          <cell r="L135" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="F136">
-            <v>511.85388891587854</v>
-          </cell>
-          <cell r="H136" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I136">
-            <v>528.77700000000004</v>
-          </cell>
-          <cell r="J136">
-            <v>526.65934037585919</v>
-          </cell>
-          <cell r="L136" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="F137">
-            <v>511.78404163500227</v>
-          </cell>
-          <cell r="H137" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I137">
-            <v>529.77700000000004</v>
-          </cell>
-          <cell r="J137">
-            <v>526.6020435225081</v>
-          </cell>
-          <cell r="L137" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="138">
-          <cell r="F138">
-            <v>511.71412112994341</v>
-          </cell>
-          <cell r="H138" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I138">
-            <v>530.77700000000004</v>
-          </cell>
-          <cell r="J138">
-            <v>526.54468650745457</v>
-          </cell>
-          <cell r="L138" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="F139">
-            <v>511.64412758496741</v>
-          </cell>
-          <cell r="H139" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I139">
-            <v>531.77700000000004</v>
-          </cell>
-          <cell r="J139">
-            <v>526.48726948179603</v>
-          </cell>
-          <cell r="L139" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="F140">
-            <v>511.57406118391361</v>
-          </cell>
-          <cell r="H140" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I140">
-            <v>532.77700000000004</v>
-          </cell>
-          <cell r="J140">
-            <v>526.42979259628146</v>
-          </cell>
-          <cell r="L140" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="F141">
-            <v>511.50392211019528</v>
-          </cell>
-          <cell r="H141" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I141">
-            <v>533.77700000000004</v>
-          </cell>
-          <cell r="J141">
-            <v>526.3722560013116</v>
-          </cell>
-          <cell r="L141" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="F142">
-            <v>511.43371054679989</v>
-          </cell>
-          <cell r="H142" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I142">
-            <v>534.77700000000004</v>
-          </cell>
-          <cell r="J142">
-            <v>526.31465984693955</v>
-          </cell>
-          <cell r="L142" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="F143">
-            <v>511.36342667628918</v>
-          </cell>
-          <cell r="H143" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I143">
-            <v>535.77700000000004</v>
-          </cell>
-          <cell r="J143">
-            <v>526.25700428287041</v>
-          </cell>
-          <cell r="L143" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="F144">
-            <v>511.29307068079947</v>
-          </cell>
-          <cell r="H144" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I144">
-            <v>536.77700000000004</v>
-          </cell>
-          <cell r="J144">
-            <v>526.19928945846152</v>
-          </cell>
-          <cell r="L144" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="F145">
-            <v>511.22264274204184</v>
-          </cell>
-          <cell r="H145" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I145">
-            <v>537.77700000000004</v>
-          </cell>
-          <cell r="J145">
-            <v>526.14151552272301</v>
-          </cell>
-          <cell r="L145" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="F146">
-            <v>511.15214304130234</v>
-          </cell>
-          <cell r="H146" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I146">
-            <v>538.77700000000004</v>
-          </cell>
-          <cell r="J146">
-            <v>526.08368262431736</v>
-          </cell>
-          <cell r="L146" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="F147">
-            <v>511.08157175944228</v>
-          </cell>
-          <cell r="H147" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I147">
-            <v>539.77700000000004</v>
-          </cell>
-          <cell r="J147">
-            <v>526.02579091156008</v>
-          </cell>
-          <cell r="L147" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="F148">
-            <v>511.01092907689838</v>
-          </cell>
-          <cell r="H148" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I148">
-            <v>540.77700000000004</v>
-          </cell>
-          <cell r="J148">
-            <v>525.96784053241993</v>
-          </cell>
-          <cell r="L148" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="F149">
-            <v>510.9402151736831</v>
-          </cell>
-          <cell r="H149" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I149">
-            <v>541.77700000000004</v>
-          </cell>
-          <cell r="J149">
-            <v>525.9098316345187</v>
-          </cell>
-          <cell r="L149" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="F150">
-            <v>510.86943022938488</v>
-          </cell>
-          <cell r="H150" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I150">
-            <v>542.77700000000004</v>
-          </cell>
-          <cell r="J150">
-            <v>525.85176436513154</v>
-          </cell>
-          <cell r="L150" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="F151">
-            <v>510.79857442316825</v>
-          </cell>
-          <cell r="H151" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I151">
-            <v>543.77700000000004</v>
-          </cell>
-          <cell r="J151">
-            <v>525.79363887118745</v>
-          </cell>
-          <cell r="L151" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="F152">
-            <v>510.72764793377445</v>
-          </cell>
-          <cell r="H152" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I152">
-            <v>544.77700000000004</v>
-          </cell>
-          <cell r="J152">
-            <v>525.73545529926946</v>
-          </cell>
-          <cell r="L152" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="F153">
-            <v>510.65665093952134</v>
-          </cell>
-          <cell r="H153" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I153">
-            <v>545.77700000000004</v>
-          </cell>
-          <cell r="J153">
-            <v>525.67721379561419</v>
-          </cell>
-          <cell r="L153" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="F154">
-            <v>510.58558361830382</v>
-          </cell>
-          <cell r="H154" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I154">
-            <v>546.77700000000004</v>
-          </cell>
-          <cell r="J154">
-            <v>525.61891450611313</v>
-          </cell>
-          <cell r="L154" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="F155">
-            <v>510.5144461475943</v>
-          </cell>
-          <cell r="H155" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I155">
-            <v>547.77700000000004</v>
-          </cell>
-          <cell r="J155">
-            <v>525.56055757631214</v>
-          </cell>
-          <cell r="L155" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="F156">
-            <v>510.44323870444265</v>
-          </cell>
-          <cell r="H156" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I156">
-            <v>548.77700000000004</v>
-          </cell>
-          <cell r="J156">
-            <v>525.5021431514117</v>
-          </cell>
-          <cell r="L156" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="F157">
-            <v>510.37196146547694</v>
-          </cell>
-          <cell r="H157" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I157">
-            <v>549.77700000000004</v>
-          </cell>
-          <cell r="J157">
-            <v>525.4436713762675</v>
-          </cell>
-          <cell r="L157" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="F158">
-            <v>510.30061460690325</v>
-          </cell>
-          <cell r="H158" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I158">
-            <v>550.77700000000004</v>
-          </cell>
-          <cell r="J158">
-            <v>525.38514239539063</v>
-          </cell>
-          <cell r="L158" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="F159">
-            <v>510.2291983045065</v>
-          </cell>
-          <cell r="H159" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I159">
-            <v>551.77700000000004</v>
-          </cell>
-          <cell r="J159">
-            <v>525.32655635294759</v>
-          </cell>
-          <cell r="L159" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="F160">
-            <v>510.15771273365044</v>
-          </cell>
-          <cell r="H160" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I160">
-            <v>552.77700000000004</v>
-          </cell>
-          <cell r="J160">
-            <v>525.26791339276087</v>
-          </cell>
-          <cell r="L160" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="F161">
-            <v>510.08615806927816</v>
-          </cell>
-          <cell r="H161" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I161">
-            <v>553.77700000000004</v>
-          </cell>
-          <cell r="J161">
-            <v>525.20921365830861</v>
-          </cell>
-          <cell r="L161" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="F162">
-            <v>510.01453448591224</v>
-          </cell>
-          <cell r="H162" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I162">
-            <v>554.77700000000004</v>
-          </cell>
-          <cell r="J162">
-            <v>525.15045729272595</v>
-          </cell>
-          <cell r="L162" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="F163">
-            <v>509.94284215765532</v>
-          </cell>
-          <cell r="H163" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I163">
-            <v>555.77700000000004</v>
-          </cell>
-          <cell r="J163">
-            <v>525.09164443880434</v>
-          </cell>
-          <cell r="L163" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="F164">
-            <v>509.87108125819049</v>
-          </cell>
-          <cell r="H164" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I164">
-            <v>556.77700000000004</v>
-          </cell>
-          <cell r="J164">
-            <v>525.03277523899203</v>
-          </cell>
-          <cell r="L164" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="F165">
-            <v>509.79925196078131</v>
-          </cell>
-          <cell r="H165" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I165">
-            <v>557.77700000000004</v>
-          </cell>
-          <cell r="J165">
-            <v>524.97384983539496</v>
-          </cell>
-          <cell r="L165" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="166">
-          <cell r="F166">
-            <v>509.72735443827258</v>
-          </cell>
-          <cell r="H166" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I166">
-            <v>558.77700000000004</v>
-          </cell>
-          <cell r="J166">
-            <v>524.91486836977606</v>
-          </cell>
-          <cell r="L166" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="F167">
-            <v>509.65538886309048</v>
-          </cell>
-          <cell r="H167" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I167">
-            <v>559.77700000000004</v>
-          </cell>
-          <cell r="J167">
-            <v>524.85583098355642</v>
-          </cell>
-          <cell r="L167" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="F168">
-            <v>509.58335540724306</v>
-          </cell>
-          <cell r="H168" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I168">
-            <v>560.77700000000004</v>
-          </cell>
-          <cell r="J168">
-            <v>524.79673781781537</v>
-          </cell>
-          <cell r="L168" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="169">
-          <cell r="F169">
-            <v>509.51125424232055</v>
-          </cell>
-          <cell r="H169" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I169">
-            <v>561.77700000000004</v>
-          </cell>
-          <cell r="J169">
-            <v>524.73758901329029</v>
-          </cell>
-          <cell r="L169" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="170">
-          <cell r="F170">
-            <v>509.43908553949586</v>
-          </cell>
-          <cell r="H170" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I170">
-            <v>562.77700000000004</v>
-          </cell>
-          <cell r="J170">
-            <v>524.67838471037794</v>
-          </cell>
-          <cell r="L170" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="171">
-          <cell r="F171">
-            <v>509.36684946952499</v>
-          </cell>
-          <cell r="H171" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I171">
-            <v>563.77700000000004</v>
-          </cell>
-          <cell r="J171">
-            <v>524.61912504913346</v>
-          </cell>
-          <cell r="L171" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="172">
-          <cell r="F172">
-            <v>509.29454620274726</v>
-          </cell>
-          <cell r="H172" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I172">
-            <v>564.77700000000004</v>
-          </cell>
-          <cell r="J172">
-            <v>524.55981016927217</v>
-          </cell>
-          <cell r="L172" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="173">
-          <cell r="F173">
-            <v>509.22217590908588</v>
-          </cell>
-          <cell r="H173" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I173">
-            <v>565.77700000000004</v>
-          </cell>
-          <cell r="J173">
-            <v>524.50044021016845</v>
-          </cell>
-          <cell r="L173" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="174">
-          <cell r="F174">
-            <v>509.14973875804844</v>
-          </cell>
-          <cell r="H174" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I174">
-            <v>566.77700000000004</v>
-          </cell>
-          <cell r="J174">
-            <v>524.44101531085732</v>
-          </cell>
-          <cell r="L174" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="175">
-          <cell r="F175">
-            <v>509.07723491872719</v>
-          </cell>
-          <cell r="H175" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I175">
-            <v>567.77700000000004</v>
-          </cell>
-          <cell r="J175">
-            <v>524.38153561003412</v>
-          </cell>
-          <cell r="L175" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="176">
-          <cell r="F176">
-            <v>509.00466455979949</v>
-          </cell>
-          <cell r="H176" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I176">
-            <v>568.77700000000004</v>
-          </cell>
-          <cell r="J176">
-            <v>524.32200124605492</v>
-          </cell>
-          <cell r="L176" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="177">
-          <cell r="F177">
-            <v>508.93202784952831</v>
-          </cell>
-          <cell r="H177" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I177">
-            <v>569.77700000000004</v>
-          </cell>
-          <cell r="J177">
-            <v>524.26241235693692</v>
-          </cell>
-          <cell r="L177" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="178">
-          <cell r="F178">
-            <v>508.85932495576276</v>
-          </cell>
-          <cell r="H178" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I178">
-            <v>570.77700000000004</v>
-          </cell>
-          <cell r="J178">
-            <v>524.20276908035896</v>
-          </cell>
-          <cell r="L178" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="179">
-          <cell r="F179">
-            <v>508.78655604593837</v>
-          </cell>
-          <cell r="H179" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I179">
-            <v>571.77700000000004</v>
-          </cell>
-          <cell r="J179">
-            <v>524.14307155366168</v>
-          </cell>
-          <cell r="L179" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="180">
-          <cell r="F180">
-            <v>508.71372128707765</v>
-          </cell>
-          <cell r="H180" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I180">
-            <v>572.77700000000004</v>
-          </cell>
-          <cell r="J180">
-            <v>524.08331991384807</v>
-          </cell>
-          <cell r="L180" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="181">
-          <cell r="F181">
-            <v>508.64082084579047</v>
-          </cell>
-          <cell r="H181" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I181">
-            <v>573.77700000000004</v>
-          </cell>
-          <cell r="J181">
-            <v>524.0235142975838</v>
-          </cell>
-          <cell r="L181" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="182">
-          <cell r="F182">
-            <v>508.56785488827472</v>
-          </cell>
-          <cell r="H182" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I182">
-            <v>574.77700000000004</v>
-          </cell>
-          <cell r="J182">
-            <v>523.96365484119724</v>
-          </cell>
-          <cell r="L182" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="183">
-          <cell r="F183">
-            <v>508.49482358031651</v>
-          </cell>
-          <cell r="H183" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I183">
-            <v>575.77700000000004</v>
-          </cell>
-          <cell r="J183">
-            <v>523.90374168068058</v>
-          </cell>
-          <cell r="L183" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="184">
-          <cell r="F184">
-            <v>508.42172708729095</v>
-          </cell>
-          <cell r="H184" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I184">
-            <v>576.77700000000004</v>
-          </cell>
-          <cell r="J184">
-            <v>523.8437749516894</v>
-          </cell>
-          <cell r="L184" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="185">
-          <cell r="F185">
-            <v>508.34856557416231</v>
-          </cell>
-          <cell r="H185" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I185">
-            <v>577.77700000000004</v>
-          </cell>
-          <cell r="J185">
-            <v>523.78375478954376</v>
-          </cell>
-          <cell r="L185" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="186">
-          <cell r="F186">
-            <v>508.27533920548484</v>
-          </cell>
-          <cell r="H186" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I186">
-            <v>578.77700000000004</v>
-          </cell>
-          <cell r="J186">
-            <v>523.72368132922827</v>
-          </cell>
-          <cell r="L186" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="187">
-          <cell r="F187">
-            <v>508.20204814540307</v>
-          </cell>
-          <cell r="H187" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I187">
-            <v>579.77700000000004</v>
-          </cell>
-          <cell r="J187">
-            <v>523.66355470539224</v>
-          </cell>
-          <cell r="L187" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="188">
-          <cell r="F188">
-            <v>508.12869255765241</v>
-          </cell>
-          <cell r="H188" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I188">
-            <v>580.77700000000004</v>
-          </cell>
-          <cell r="J188">
-            <v>523.60337505235066</v>
-          </cell>
-          <cell r="L188" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="189">
-          <cell r="F189">
-            <v>508.05527260555948</v>
-          </cell>
-          <cell r="H189" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I189">
-            <v>581.77700000000004</v>
-          </cell>
-          <cell r="J189">
-            <v>523.54314250408424</v>
-          </cell>
-          <cell r="L189" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="190">
-          <cell r="F190">
-            <v>507.98178845204291</v>
-          </cell>
-          <cell r="H190" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I190">
-            <v>582.77700000000004</v>
-          </cell>
-          <cell r="J190">
-            <v>523.48285719423973</v>
-          </cell>
-          <cell r="L190" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="191">
-          <cell r="F191">
-            <v>507.90824025961354</v>
-          </cell>
-          <cell r="H191" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I191">
-            <v>583.77700000000004</v>
-          </cell>
-          <cell r="J191">
-            <v>523.42251925613073</v>
-          </cell>
-          <cell r="L191" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="192">
-          <cell r="F192">
-            <v>507.83462819037521</v>
-          </cell>
-          <cell r="H192" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I192">
-            <v>584.77700000000004</v>
-          </cell>
-          <cell r="J192">
-            <v>523.36212882273765</v>
-          </cell>
-          <cell r="L192" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="193">
-          <cell r="F193">
-            <v>507.76095240602518</v>
-          </cell>
-          <cell r="H193" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I193">
-            <v>585.77700000000004</v>
-          </cell>
-          <cell r="J193">
-            <v>523.30168602670869</v>
-          </cell>
-          <cell r="L193" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="194">
-          <cell r="F194">
-            <v>507.68721306785454</v>
-          </cell>
-          <cell r="H194" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I194">
-            <v>586.77700000000004</v>
-          </cell>
-          <cell r="J194">
-            <v>523.24119100035955</v>
-          </cell>
-          <cell r="L194" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="195">
-          <cell r="F195">
-            <v>507.6134103367491</v>
-          </cell>
-          <cell r="H195" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I195">
-            <v>587.77700000000004</v>
-          </cell>
-          <cell r="J195">
-            <v>523.18064387567472</v>
-          </cell>
-          <cell r="L195" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="196">
-          <cell r="F196">
-            <v>507.53954437318941</v>
-          </cell>
-          <cell r="H196" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I196">
-            <v>588.77700000000004</v>
-          </cell>
-          <cell r="J196">
-            <v>523.12004478430697</v>
-          </cell>
-          <cell r="L196" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="197">
-          <cell r="F197">
-            <v>507.46561533725185</v>
-          </cell>
-          <cell r="H197" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I197">
-            <v>589.77700000000004</v>
-          </cell>
-          <cell r="J197">
-            <v>523.0593938575787</v>
-          </cell>
-          <cell r="L197" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="198">
-          <cell r="F198">
-            <v>507.39162338860876</v>
-          </cell>
-          <cell r="H198" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I198">
-            <v>590.77700000000004</v>
-          </cell>
-          <cell r="J198">
-            <v>522.99869122648181</v>
-          </cell>
-          <cell r="L198" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="199">
-          <cell r="F199">
-            <v>507.31756868652928</v>
-          </cell>
-          <cell r="H199" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I199">
-            <v>591.77700000000004</v>
-          </cell>
-          <cell r="J199">
-            <v>522.93793702167818</v>
-          </cell>
-          <cell r="L199" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="200">
-          <cell r="F200">
-            <v>507.24345138987974</v>
-          </cell>
-          <cell r="H200" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I200">
-            <v>592.77700000000004</v>
-          </cell>
-          <cell r="J200">
-            <v>522.87713137350056</v>
-          </cell>
-          <cell r="L200" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="201">
-          <cell r="F201">
-            <v>507.16927165712428</v>
-          </cell>
-          <cell r="H201" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I201">
-            <v>593.77700000000004</v>
-          </cell>
-          <cell r="J201">
-            <v>522.81627441195235</v>
-          </cell>
-          <cell r="L201" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="202">
-          <cell r="F202">
-            <v>507.09502964632537</v>
-          </cell>
-          <cell r="H202" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I202">
-            <v>594.77700000000004</v>
-          </cell>
-          <cell r="J202">
-            <v>522.75536626670873</v>
-          </cell>
-          <cell r="L202" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="203">
-          <cell r="F203">
-            <v>507.02072551514453</v>
-          </cell>
-          <cell r="H203" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I203">
-            <v>595.77700000000004</v>
-          </cell>
-          <cell r="J203">
-            <v>522.69440706711669</v>
-          </cell>
-          <cell r="L203" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="204">
-          <cell r="F204">
-            <v>506.94635942084278</v>
-          </cell>
-          <cell r="H204" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I204">
-            <v>596.77700000000004</v>
-          </cell>
-          <cell r="J204">
-            <v>522.63339694219565</v>
-          </cell>
-          <cell r="L204" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="205">
-          <cell r="F205">
-            <v>506.87193152028112</v>
-          </cell>
-          <cell r="H205" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I205">
-            <v>597.77700000000004</v>
-          </cell>
-          <cell r="J205">
-            <v>522.57233602063775</v>
-          </cell>
-          <cell r="L205" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="206">
-          <cell r="F206">
-            <v>506.79744196992141</v>
-          </cell>
-          <cell r="H206" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I206">
-            <v>598.77700000000004</v>
-          </cell>
-          <cell r="J206">
-            <v>522.51122443080885</v>
-          </cell>
-          <cell r="L206" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="207">
-          <cell r="F207">
-            <v>506.72289092582673</v>
-          </cell>
-          <cell r="H207" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I207">
-            <v>599.77700000000004</v>
-          </cell>
-          <cell r="J207">
-            <v>522.45006230074841</v>
-          </cell>
-          <cell r="L207" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="208">
-          <cell r="F208">
-            <v>506.648278543662</v>
-          </cell>
-          <cell r="H208" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I208">
-            <v>600.77700000000004</v>
-          </cell>
-          <cell r="J208">
-            <v>522.38884975816995</v>
-          </cell>
-          <cell r="L208" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="209">
-          <cell r="F209">
-            <v>506.57360497869468</v>
-          </cell>
-          <cell r="H209" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I209">
-            <v>601.77700000000004</v>
-          </cell>
-          <cell r="J209">
-            <v>522.3275869304623</v>
-          </cell>
-          <cell r="L209" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="210">
-          <cell r="F210">
-            <v>506.49887038579521</v>
-          </cell>
-          <cell r="H210" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I210">
-            <v>602.77700000000004</v>
-          </cell>
-          <cell r="J210">
-            <v>522.26627394468937</v>
-          </cell>
-          <cell r="L210" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="211">
-          <cell r="F211">
-            <v>506.42407491943789</v>
-          </cell>
-          <cell r="H211" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I211">
-            <v>603.77700000000004</v>
-          </cell>
-          <cell r="J211">
-            <v>522.2049109275905</v>
-          </cell>
-          <cell r="L211" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="212">
-          <cell r="F212">
-            <v>506.34921873370104</v>
-          </cell>
-          <cell r="H212" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I212">
-            <v>604.77700000000004</v>
-          </cell>
-          <cell r="J212">
-            <v>522.14349800558182</v>
-          </cell>
-          <cell r="L212" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="213">
-          <cell r="F213">
-            <v>506.27430198226807</v>
-          </cell>
-          <cell r="H213" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I213">
-            <v>605.77700000000004</v>
-          </cell>
-          <cell r="J213">
-            <v>522.08203530475578</v>
-          </cell>
-          <cell r="L213" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="214">
-          <cell r="F214">
-            <v>506.1993248184279</v>
-          </cell>
-          <cell r="H214" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I214">
-            <v>606.77700000000004</v>
-          </cell>
-          <cell r="J214">
-            <v>522.02052295088254</v>
-          </cell>
-          <cell r="L214" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="215">
-          <cell r="F215">
-            <v>506.1242873950755</v>
-          </cell>
-          <cell r="H215" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I215">
-            <v>607.77700000000004</v>
-          </cell>
-          <cell r="J215">
-            <v>521.9589610694095</v>
-          </cell>
-          <cell r="L215" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="216">
-          <cell r="F216">
-            <v>506.04918986471262</v>
-          </cell>
-          <cell r="H216" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I216">
-            <v>608.77700000000004</v>
-          </cell>
-          <cell r="J216">
-            <v>521.89734978546278</v>
-          </cell>
-          <cell r="L216" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="217">
-          <cell r="F217">
-            <v>505.97403237944837</v>
-          </cell>
-          <cell r="H217" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I217">
-            <v>609.77700000000004</v>
-          </cell>
-          <cell r="J217">
-            <v>521.83568922384688</v>
-          </cell>
-          <cell r="L217" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="218">
-          <cell r="F218">
-            <v>505.89881509100007</v>
-          </cell>
-          <cell r="H218" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I218">
-            <v>610.77700000000004</v>
-          </cell>
-          <cell r="J218">
-            <v>521.77397950904606</v>
-          </cell>
-          <cell r="L218" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="219">
-          <cell r="F219">
-            <v>505.82353815069337</v>
-          </cell>
-          <cell r="H219" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I219">
-            <v>611.77700000000004</v>
-          </cell>
-          <cell r="J219">
-            <v>521.71222076522383</v>
-          </cell>
-          <cell r="L219" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="220">
-          <cell r="F220">
-            <v>505.74820170946339</v>
-          </cell>
-          <cell r="H220" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I220">
-            <v>612.77700000000004</v>
-          </cell>
-          <cell r="J220">
-            <v>521.65041311622429</v>
-          </cell>
-          <cell r="L220" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="221">
-          <cell r="F221">
-            <v>505.67280591785521</v>
-          </cell>
-          <cell r="H221" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I221">
-            <v>613.77700000000004</v>
-          </cell>
-          <cell r="J221">
-            <v>521.58855668557248</v>
-          </cell>
-          <cell r="L221" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="222">
-          <cell r="F222">
-            <v>505.59735092602432</v>
-          </cell>
-          <cell r="H222" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I222">
-            <v>614.77700000000004</v>
-          </cell>
-          <cell r="J222">
-            <v>521.52665159647461</v>
-          </cell>
-          <cell r="L222" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="223">
-          <cell r="F223">
-            <v>505.52183688373759</v>
-          </cell>
-          <cell r="H223" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I223">
-            <v>615.77700000000004</v>
-          </cell>
-          <cell r="J223">
-            <v>521.46469797181885</v>
-          </cell>
-          <cell r="L223" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="224">
-          <cell r="F224">
-            <v>505.44626394037357</v>
-          </cell>
-          <cell r="H224" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I224">
-            <v>616.77700000000004</v>
-          </cell>
-          <cell r="J224">
-            <v>521.40269593417565</v>
-          </cell>
-          <cell r="L224" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="225">
-          <cell r="F225">
-            <v>505.37063224492351</v>
-          </cell>
-          <cell r="H225" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I225">
-            <v>617.77700000000004</v>
-          </cell>
-          <cell r="J225">
-            <v>521.34064560579861</v>
-          </cell>
-          <cell r="L225" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="226">
-          <cell r="F226">
-            <v>505.2949419459917</v>
-          </cell>
-          <cell r="H226" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I226">
-            <v>618.77700000000004</v>
-          </cell>
-          <cell r="J226">
-            <v>521.27854710862448</v>
-          </cell>
-          <cell r="L226" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="227">
-          <cell r="F227">
-            <v>505.21919319179625</v>
-          </cell>
-          <cell r="H227" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I227">
-            <v>619.77700000000004</v>
-          </cell>
-          <cell r="J227">
-            <v>521.21640056427441</v>
-          </cell>
-          <cell r="L227" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="228">
-          <cell r="F228">
-            <v>505.14338613016986</v>
-          </cell>
-          <cell r="H228" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I228">
-            <v>620.77700000000004</v>
-          </cell>
-          <cell r="J228">
-            <v>521.15420609405362</v>
-          </cell>
-          <cell r="L228" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="229">
-          <cell r="F229">
-            <v>505.06752090856025</v>
-          </cell>
-          <cell r="H229" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I229">
-            <v>621.77700000000004</v>
-          </cell>
-          <cell r="J229">
-            <v>521.09196381895276</v>
-          </cell>
-          <cell r="L229" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="230">
-          <cell r="F230">
-            <v>504.99159767403114</v>
-          </cell>
-          <cell r="H230" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I230">
-            <v>622.77700000000004</v>
-          </cell>
-          <cell r="J230">
-            <v>521.02967385964803</v>
-          </cell>
-          <cell r="L230" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="231">
-          <cell r="F231">
-            <v>504.91561657326247</v>
-          </cell>
-          <cell r="H231" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I231">
-            <v>623.77700000000004</v>
-          </cell>
-          <cell r="J231">
-            <v>520.96733633650172</v>
-          </cell>
-          <cell r="L231" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="232">
-          <cell r="F232">
-            <v>504.83957775255158</v>
-          </cell>
-          <cell r="H232" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I232">
-            <v>624.77700000000004</v>
-          </cell>
-          <cell r="J232">
-            <v>520.9049513695627</v>
-          </cell>
-          <cell r="L232" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="233">
-          <cell r="F233">
-            <v>504.76348135781359</v>
-          </cell>
-          <cell r="H233" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I233">
-            <v>625.77700000000004</v>
-          </cell>
-          <cell r="J233">
-            <v>520.84251907856719</v>
-          </cell>
-          <cell r="L233" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="234">
-          <cell r="F234">
-            <v>504.68732753458198</v>
-          </cell>
-          <cell r="H234" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I234">
-            <v>626.77700000000004</v>
-          </cell>
-          <cell r="J234">
-            <v>520.78003958293948</v>
-          </cell>
-          <cell r="L234" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="235">
-          <cell r="F235">
-            <v>504.61111642800961</v>
-          </cell>
-          <cell r="H235" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I235">
-            <v>627.77700000000004</v>
-          </cell>
-          <cell r="J235">
-            <v>520.71751300179176</v>
-          </cell>
-          <cell r="L235" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="236">
-          <cell r="F236">
-            <v>504.5348481828691</v>
-          </cell>
-          <cell r="H236" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I236">
-            <v>628.77700000000004</v>
-          </cell>
-          <cell r="J236">
-            <v>520.65493945392541</v>
-          </cell>
-          <cell r="L236" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="237">
-          <cell r="F237">
-            <v>504.4585229435537</v>
-          </cell>
-          <cell r="H237" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I237">
-            <v>629.77700000000004</v>
-          </cell>
-          <cell r="J237">
-            <v>520.59231905783099</v>
-          </cell>
-          <cell r="L237" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="238">
-          <cell r="F238">
-            <v>504.38214085407787</v>
-          </cell>
-          <cell r="H238" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I238">
-            <v>630.77700000000004</v>
-          </cell>
-          <cell r="J238">
-            <v>520.52965193168961</v>
-          </cell>
-          <cell r="L238" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="239">
-          <cell r="F239">
-            <v>504.30570205807794</v>
-          </cell>
-          <cell r="H239" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I239">
-            <v>631.77700000000004</v>
-          </cell>
-          <cell r="J239">
-            <v>520.46693819337247</v>
-          </cell>
-          <cell r="L239" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="240">
-          <cell r="F240">
-            <v>504.22920669881302</v>
-          </cell>
-          <cell r="H240" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I240">
-            <v>632.77700000000004</v>
-          </cell>
-          <cell r="J240">
-            <v>520.40417796044198</v>
-          </cell>
-          <cell r="L240" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="241">
-          <cell r="F241">
-            <v>504.1526549191654</v>
-          </cell>
-          <cell r="H241" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I241">
-            <v>633.77700000000004</v>
-          </cell>
-          <cell r="J241">
-            <v>520.34137135015249</v>
-          </cell>
-          <cell r="L241" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="242">
-          <cell r="F242">
-            <v>504.07604686164143</v>
-          </cell>
-          <cell r="H242" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I242">
-            <v>634.77700000000004</v>
-          </cell>
-          <cell r="J242">
-            <v>520.27851847945044</v>
-          </cell>
-          <cell r="L242" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="243">
-          <cell r="F243">
-            <v>503.99938266837228</v>
-          </cell>
-          <cell r="H243" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I243">
-            <v>635.77700000000004</v>
-          </cell>
-          <cell r="J243">
-            <v>520.21561946497513</v>
-          </cell>
-          <cell r="L243" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="244">
-          <cell r="F244">
-            <v>503.9226624811144</v>
-          </cell>
-          <cell r="H244" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I244">
-            <v>636.77700000000004</v>
-          </cell>
-          <cell r="J244">
-            <v>520.15267442305935</v>
-          </cell>
-          <cell r="L244" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="245">
-          <cell r="F245">
-            <v>503.8458864412504</v>
-          </cell>
-          <cell r="H245" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I245">
-            <v>637.77700000000004</v>
-          </cell>
-          <cell r="J245">
-            <v>520.08968346972961</v>
-          </cell>
-          <cell r="L245" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="246">
-          <cell r="F246">
-            <v>503.76905468978975</v>
-          </cell>
-          <cell r="H246" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I246">
-            <v>638.77700000000004</v>
-          </cell>
-          <cell r="J246">
-            <v>520.02664672070739</v>
-          </cell>
-          <cell r="L246" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="247">
-          <cell r="F247">
-            <v>503.69216736736951</v>
-          </cell>
-          <cell r="H247" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I247">
-            <v>639.77700000000004</v>
-          </cell>
-          <cell r="J247">
-            <v>519.96356429140906</v>
-          </cell>
-          <cell r="L247" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="248">
-          <cell r="F248">
-            <v>503.61522461425471</v>
-          </cell>
-          <cell r="H248" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I248">
-            <v>640.77700000000004</v>
-          </cell>
-          <cell r="J248">
-            <v>519.90043629694651</v>
-          </cell>
-          <cell r="L248" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="249">
-          <cell r="F249">
-            <v>503.53822657033976</v>
-          </cell>
-          <cell r="H249" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I249">
-            <v>641.77700000000004</v>
-          </cell>
-          <cell r="J249">
-            <v>519.83726285212845</v>
-          </cell>
-          <cell r="L249" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="250">
-          <cell r="F250">
-            <v>503.46117337514841</v>
-          </cell>
-          <cell r="H250" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I250">
-            <v>642.77700000000004</v>
-          </cell>
-          <cell r="J250">
-            <v>519.77404407145991</v>
-          </cell>
-          <cell r="L250" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="251">
-          <cell r="F251">
-            <v>503.38406516783493</v>
-          </cell>
-          <cell r="H251" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I251">
-            <v>643.77700000000004</v>
-          </cell>
-          <cell r="J251">
-            <v>519.71078006914354</v>
-          </cell>
-          <cell r="L251" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="252">
-          <cell r="F252">
-            <v>503.30690208718465</v>
-          </cell>
-          <cell r="H252" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I252">
-            <v>644.77700000000004</v>
-          </cell>
-          <cell r="J252">
-            <v>519.64747095908024</v>
-          </cell>
-          <cell r="L252" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="253">
-          <cell r="F253">
-            <v>503.22968427161481</v>
-          </cell>
-          <cell r="H253" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I253">
-            <v>645.77700000000004</v>
-          </cell>
-          <cell r="J253">
-            <v>519.58411685486908</v>
-          </cell>
-          <cell r="L253" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="254">
-          <cell r="F254">
-            <v>503.152411859175</v>
-          </cell>
-          <cell r="H254" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I254">
-            <v>646.77700000000004</v>
-          </cell>
-          <cell r="J254">
-            <v>519.52071786980889</v>
-          </cell>
-          <cell r="L254" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="255">
-          <cell r="F255">
-            <v>503.07508498754822</v>
-          </cell>
-          <cell r="H255" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I255">
-            <v>647.77700000000004</v>
-          </cell>
-          <cell r="J255">
-            <v>519.45727411689791</v>
-          </cell>
-          <cell r="L255" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="256">
-          <cell r="F256">
-            <v>502.99770379405152</v>
-          </cell>
-          <cell r="H256" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I256">
-            <v>648.77700000000004</v>
-          </cell>
-          <cell r="J256">
-            <v>519.39378570883468</v>
-          </cell>
-          <cell r="L256" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="257">
-          <cell r="F257">
-            <v>502.92026841563649</v>
-          </cell>
-          <cell r="H257" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I257">
-            <v>649.77700000000004</v>
-          </cell>
-          <cell r="J257">
-            <v>519.33025275801901</v>
-          </cell>
-          <cell r="L257" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="258">
-          <cell r="F258">
-            <v>502.84277898889025</v>
-          </cell>
-          <cell r="H258" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I258">
-            <v>650.77700000000004</v>
-          </cell>
-          <cell r="J258">
-            <v>519.26667537655203</v>
-          </cell>
-          <cell r="L258" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="259">
-          <cell r="F259">
-            <v>502.76523565003617</v>
-          </cell>
-          <cell r="H259" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I259">
-            <v>651.77700000000004</v>
-          </cell>
-          <cell r="J259">
-            <v>519.203053676237</v>
-          </cell>
-          <cell r="L259" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="260">
-          <cell r="F260">
-            <v>502.68763853493431</v>
-          </cell>
-          <cell r="H260" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I260">
-            <v>652.77700000000004</v>
-          </cell>
-          <cell r="J260">
-            <v>519.13938776858026</v>
-          </cell>
-          <cell r="L260" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-        <row r="261">
-          <cell r="F261">
-            <v>502.60998777908253</v>
-          </cell>
-          <cell r="H261" t="e">
-            <v>#NUM!</v>
-          </cell>
-          <cell r="I261">
-            <v>653.77700000000004</v>
-          </cell>
-          <cell r="J261">
-            <v>519.07567776479118</v>
-          </cell>
-          <cell r="L261" t="e">
-            <v>#NUM!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4877,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="N68" sqref="N68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18612,7 +14213,7 @@
         <v>3066</v>
       </c>
       <c r="B339" s="2">
-        <f t="shared" ref="B339:B402" si="58">FOCUS-(SQRT(POWER(VERTEX_V1,2)*(1+(POWER(A339,2)/POWER(B_V1,2))))*$J$1)</f>
+        <f t="shared" ref="B339:B350" si="58">FOCUS-(SQRT(POWER(VERTEX_V1,2)*(1+(POWER(A339,2)/POWER(B_V1,2))))*$J$1)</f>
         <v>479.44110994117239</v>
       </c>
       <c r="E339">
@@ -18620,7 +14221,7 @@
         <v>3066</v>
       </c>
       <c r="F339" s="2">
-        <f t="shared" ref="F339:F402" si="59">FOCUS-(SQRT(POWER(VERTEX_V2,2)*(1+(POWER($B$1-E339,2)/POWER(B_V2,2))))*$J$2)</f>
+        <f t="shared" ref="F339:F350" si="59">FOCUS-(SQRT(POWER(VERTEX_V2,2)*(1+(POWER($B$1-E339,2)/POWER(B_V2,2))))*$J$2)</f>
         <v>600.70002101114017</v>
       </c>
       <c r="G339" s="4">
@@ -18628,7 +14229,7 @@
         <v>121.25891106996778</v>
       </c>
       <c r="J339" s="2">
-        <f t="shared" ref="J339:J402" si="61">FOCUS+(SQRT(POWER(VERTEX_H1,2)*(1+(POWER(K339,2)/POWER(B_H1,2))))*$J$3)</f>
+        <f t="shared" ref="J339:J350" si="61">FOCUS+(SQRT(POWER(VERTEX_H1,2)*(1+(POWER(K339,2)/POWER(B_H1,2))))*$J$3)</f>
         <v>-76.770871985597182</v>
       </c>
       <c r="K339">
@@ -18636,7 +14237,7 @@
         <v>3201</v>
       </c>
       <c r="N339" s="2">
-        <f t="shared" ref="N339:N402" si="62">FOCUS+(SQRT(POWER(VERTEX_H2,2)*(1+(POWER($B$1-O339,2)/POWER(B_H2,2))))*$J$4)</f>
+        <f t="shared" ref="N339:N350" si="62">FOCUS+(SQRT(POWER(VERTEX_H2,2)*(1+(POWER($B$1-O339,2)/POWER(B_H2,2))))*$J$4)</f>
         <v>197.22030462666902</v>
       </c>
       <c r="O339">
@@ -19117,14 +14718,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1">
+        <v>120000000</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="7">
+        <f>1/(B1/B2)</f>
+        <v>6.6666666666666668E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>343</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <f>(B4*1000)*B3</f>
+        <v>2.2866666666666667E-2</v>
+      </c>
+      <c r="D5">
+        <f>B5*14</f>
+        <v>0.32013333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>300/B5</f>
+        <v>13119.533527696793</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>B6/2</f>
+        <v>6559.7667638483963</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>13120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>B9/2</f>
+        <v>6560</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f>SQRT(POWER(B9,2)*2)</f>
+        <v>18554.481938335008</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>